<commit_message>
LSTM optimized, training with different hyperparameters complete
</commit_message>
<xml_diff>
--- a/LSTM report.xlsx
+++ b/LSTM report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yixin\Desktop\Workspace\University\MSc\Machine Learning for Quantified Self\MLQS-VU-Project-Tyson\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{10A42C7D-9E0C-4AB7-88B4-FBD3E7229DA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{FBB49DA9-EDAB-4148-9FD8-9DBD41DB207A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="17520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="17">
   <si>
     <t>Trial</t>
   </si>
@@ -45,12 +45,6 @@
   </si>
   <si>
     <t>Overall Accuracy</t>
-  </si>
-  <si>
-    <t>Window size 50</t>
-  </si>
-  <si>
-    <t>Window size 100</t>
   </si>
   <si>
     <t>Epochs=1000 for all models</t>
@@ -83,14 +77,23 @@
     <t>Stopped at Epochs No.</t>
   </si>
   <si>
-    <t>Number of layers</t>
+    <t>Number of hidden layers</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>sequencial data at window 50</t>
+  </si>
+  <si>
+    <t>sequencial data at window 100</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,6 +111,11 @@
     </font>
     <font>
       <sz val="7"/>
+      <color theme="1"/>
+      <name val="Var(--jp-code-font-family)"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Var(--jp-code-font-family)"/>
     </font>
@@ -147,14 +155,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -164,15 +169,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -488,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:S107"/>
+  <dimension ref="B2:S155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="T111" sqref="T111"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -501,13 +505,15 @@
   <sheetData>
     <row r="2" spans="2:19">
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:19">
-      <c r="B4" s="2"/>
+      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="C4" s="3" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -515,98 +521,98 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+    </row>
+    <row r="5" spans="2:19">
+      <c r="B5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4">
+        <v>2</v>
+      </c>
+      <c r="E5" s="4">
+        <v>3</v>
+      </c>
+      <c r="F5" s="4">
         <v>4</v>
       </c>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-    </row>
-    <row r="5" spans="2:19">
-      <c r="B5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="5">
-        <v>1</v>
-      </c>
-      <c r="D5" s="5">
+      <c r="G5" s="4">
+        <v>5</v>
+      </c>
+      <c r="H5" s="4">
+        <v>6</v>
+      </c>
+      <c r="I5" s="4">
+        <v>1</v>
+      </c>
+      <c r="J5" s="4">
         <v>2</v>
       </c>
-      <c r="E5" s="5">
+      <c r="K5" s="4">
         <v>3</v>
       </c>
-      <c r="F5" s="5">
+      <c r="L5" s="4">
         <v>4</v>
       </c>
-      <c r="G5" s="5">
-        <v>5</v>
-      </c>
-      <c r="H5" s="5">
+      <c r="M5" s="4">
+        <v>5</v>
+      </c>
+      <c r="N5" s="4">
         <v>6</v>
       </c>
-      <c r="I5" s="5">
-        <v>1</v>
-      </c>
-      <c r="J5" s="5">
+    </row>
+    <row r="6" spans="2:19" ht="40" customHeight="1">
+      <c r="B6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2">
+        <v>3</v>
+      </c>
+      <c r="D6" s="2">
+        <v>3</v>
+      </c>
+      <c r="E6" s="2">
+        <v>3</v>
+      </c>
+      <c r="F6" s="2">
         <v>2</v>
       </c>
-      <c r="K5" s="5">
+      <c r="G6" s="2">
+        <v>2</v>
+      </c>
+      <c r="H6" s="2">
+        <v>2</v>
+      </c>
+      <c r="I6" s="2">
         <v>3</v>
       </c>
-      <c r="L5" s="5">
-        <v>4</v>
-      </c>
-      <c r="M5" s="5">
-        <v>5</v>
-      </c>
-      <c r="N5" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="2:19">
-      <c r="B6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="10">
+      <c r="J6" s="2">
         <v>3</v>
       </c>
-      <c r="D6" s="10">
+      <c r="K6" s="2">
         <v>3</v>
       </c>
-      <c r="E6" s="10">
-        <v>3</v>
-      </c>
-      <c r="F6" s="10">
+      <c r="L6" s="2">
         <v>2</v>
       </c>
-      <c r="G6" s="10">
+      <c r="M6" s="2">
         <v>2</v>
       </c>
-      <c r="H6" s="10">
+      <c r="N6" s="2">
         <v>2</v>
       </c>
-      <c r="I6" s="10">
-        <v>3</v>
-      </c>
-      <c r="J6" s="10">
-        <v>3</v>
-      </c>
-      <c r="K6" s="10">
-        <v>3</v>
-      </c>
-      <c r="L6" s="10">
-        <v>2</v>
-      </c>
-      <c r="M6" s="10">
-        <v>2</v>
-      </c>
-      <c r="N6" s="10">
-        <v>2</v>
-      </c>
     </row>
     <row r="7" spans="2:19">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="2">
@@ -647,8 +653,8 @@
       </c>
     </row>
     <row r="8" spans="2:19" ht="17" customHeight="1">
-      <c r="B8" s="5" t="s">
-        <v>13</v>
+      <c r="B8" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="C8" s="2">
         <v>0.5</v>
@@ -688,8 +694,8 @@
       </c>
     </row>
     <row r="9" spans="2:19" ht="25" customHeight="1">
-      <c r="B9" s="11" t="s">
-        <v>14</v>
+      <c r="B9" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="C9" s="2">
         <v>60</v>
@@ -729,13 +735,13 @@
       </c>
     </row>
     <row r="10" spans="2:19">
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="2">
         <v>0.87080000000000002</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="2">
         <v>0.80400000000000005</v>
       </c>
       <c r="E10" s="2">
@@ -750,10 +756,10 @@
       <c r="H10" s="2">
         <v>0.82410000000000005</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="2">
         <v>0.79359999999999997</v>
       </c>
-      <c r="J10" s="7">
+      <c r="J10" s="2">
         <v>0.88070000000000004</v>
       </c>
       <c r="K10" s="2">
@@ -771,42 +777,42 @@
     </row>
     <row r="14" spans="2:19">
       <c r="B14" s="1"/>
-      <c r="H14" s="9"/>
+      <c r="H14" s="7"/>
     </row>
     <row r="15" spans="2:19">
-      <c r="B15" s="7"/>
+      <c r="B15" s="6"/>
       <c r="D15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" t="s">
         <v>6</v>
       </c>
-      <c r="E15" t="s">
+      <c r="G15" t="s">
         <v>7</v>
       </c>
-      <c r="F15" t="s">
-        <v>8</v>
-      </c>
-      <c r="G15" t="s">
-        <v>9</v>
-      </c>
-      <c r="O15" s="7"/>
+      <c r="O15" s="6"/>
       <c r="P15" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>5</v>
+      </c>
+      <c r="R15" t="s">
         <v>6</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="S15" t="s">
         <v>7</v>
       </c>
-      <c r="R15" t="s">
-        <v>8</v>
-      </c>
-      <c r="S15" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="16" spans="2:19">
-      <c r="B16" s="6"/>
-      <c r="O16" s="6"/>
+      <c r="B16" s="5"/>
+      <c r="O16" s="5"/>
     </row>
     <row r="17" spans="2:19">
-      <c r="B17" s="7"/>
+      <c r="B17" s="6"/>
       <c r="C17">
         <v>0</v>
       </c>
@@ -839,7 +845,7 @@
       </c>
     </row>
     <row r="18" spans="2:19">
-      <c r="B18" s="7"/>
+      <c r="B18" s="6"/>
       <c r="C18">
         <v>1</v>
       </c>
@@ -872,7 +878,7 @@
       </c>
     </row>
     <row r="19" spans="2:19">
-      <c r="B19" s="7"/>
+      <c r="B19" s="6"/>
       <c r="C19">
         <v>2</v>
       </c>
@@ -905,7 +911,7 @@
       </c>
     </row>
     <row r="20" spans="2:19">
-      <c r="B20" s="7"/>
+      <c r="B20" s="6"/>
       <c r="C20">
         <v>3</v>
       </c>
@@ -938,7 +944,7 @@
       </c>
     </row>
     <row r="21" spans="2:19">
-      <c r="B21" s="7"/>
+      <c r="B21" s="6"/>
       <c r="C21">
         <v>4</v>
       </c>
@@ -971,7 +977,7 @@
       </c>
     </row>
     <row r="22" spans="2:19">
-      <c r="B22" s="7"/>
+      <c r="B22" s="6"/>
       <c r="C22">
         <v>5</v>
       </c>
@@ -1004,7 +1010,7 @@
       </c>
     </row>
     <row r="23" spans="2:19">
-      <c r="B23" s="7"/>
+      <c r="B23" s="6"/>
       <c r="C23">
         <v>6</v>
       </c>
@@ -1037,7 +1043,7 @@
       </c>
     </row>
     <row r="24" spans="2:19">
-      <c r="B24" s="7"/>
+      <c r="B24" s="6"/>
       <c r="C24">
         <v>7</v>
       </c>
@@ -1070,13 +1076,13 @@
       </c>
     </row>
     <row r="25" spans="2:19">
-      <c r="B25" s="6"/>
-      <c r="O25" s="6"/>
+      <c r="B25" s="5"/>
+      <c r="O25" s="5"/>
     </row>
     <row r="26" spans="2:19">
-      <c r="B26" s="7"/>
-      <c r="C26" s="9" t="s">
-        <v>10</v>
+      <c r="B26" s="6"/>
+      <c r="C26" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="F26">
         <v>0.87</v>
@@ -1084,8 +1090,8 @@
       <c r="G26">
         <v>449</v>
       </c>
-      <c r="O26" s="9" t="s">
-        <v>10</v>
+      <c r="O26" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="R26">
         <v>0.79</v>
@@ -1095,9 +1101,9 @@
       </c>
     </row>
     <row r="27" spans="2:19">
-      <c r="B27" s="7"/>
-      <c r="C27" s="9" t="s">
-        <v>11</v>
+      <c r="B27" s="6"/>
+      <c r="C27" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="D27">
         <v>0.88</v>
@@ -1111,8 +1117,8 @@
       <c r="G27">
         <v>449</v>
       </c>
-      <c r="O27" s="9" t="s">
-        <v>11</v>
+      <c r="O27" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="P27">
         <v>0.8</v>
@@ -1128,9 +1134,9 @@
       </c>
     </row>
     <row r="28" spans="2:19">
-      <c r="B28" s="7"/>
-      <c r="C28" s="9" t="s">
-        <v>12</v>
+      <c r="B28" s="6"/>
+      <c r="C28" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="D28">
         <v>0.88</v>
@@ -1144,8 +1150,8 @@
       <c r="G28">
         <v>449</v>
       </c>
-      <c r="O28" s="9" t="s">
-        <v>12</v>
+      <c r="O28" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="P28">
         <v>0.8</v>
@@ -1162,33 +1168,33 @@
     </row>
     <row r="31" spans="2:19">
       <c r="D31" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" t="s">
+        <v>5</v>
+      </c>
+      <c r="F31" t="s">
         <v>6</v>
       </c>
-      <c r="E31" t="s">
+      <c r="G31" t="s">
         <v>7</v>
       </c>
-      <c r="F31" t="s">
-        <v>8</v>
-      </c>
-      <c r="G31" t="s">
-        <v>9</v>
-      </c>
-      <c r="N31" s="7"/>
+      <c r="N31" s="6"/>
       <c r="P31" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>5</v>
+      </c>
+      <c r="R31" t="s">
         <v>6</v>
       </c>
-      <c r="Q31" t="s">
+      <c r="S31" t="s">
         <v>7</v>
       </c>
-      <c r="R31" t="s">
-        <v>8</v>
-      </c>
-      <c r="S31" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="32" spans="2:19">
-      <c r="N32" s="6"/>
+      <c r="N32" s="5"/>
     </row>
     <row r="33" spans="2:19">
       <c r="C33">
@@ -1206,7 +1212,7 @@
       <c r="G33">
         <v>57</v>
       </c>
-      <c r="N33" s="7"/>
+      <c r="N33" s="6"/>
       <c r="O33">
         <v>0</v>
       </c>
@@ -1239,7 +1245,7 @@
       <c r="G34">
         <v>66</v>
       </c>
-      <c r="N34" s="7"/>
+      <c r="N34" s="6"/>
       <c r="O34">
         <v>1</v>
       </c>
@@ -1272,7 +1278,7 @@
       <c r="G35">
         <v>72</v>
       </c>
-      <c r="N35" s="7"/>
+      <c r="N35" s="6"/>
       <c r="O35">
         <v>2</v>
       </c>
@@ -1305,7 +1311,7 @@
       <c r="G36">
         <v>52</v>
       </c>
-      <c r="N36" s="7"/>
+      <c r="N36" s="6"/>
       <c r="O36">
         <v>3</v>
       </c>
@@ -1338,7 +1344,7 @@
       <c r="G37">
         <v>51</v>
       </c>
-      <c r="N37" s="7"/>
+      <c r="N37" s="6"/>
       <c r="O37">
         <v>4</v>
       </c>
@@ -1371,7 +1377,7 @@
       <c r="G38">
         <v>53</v>
       </c>
-      <c r="N38" s="7"/>
+      <c r="N38" s="6"/>
       <c r="O38">
         <v>5</v>
       </c>
@@ -1404,7 +1410,7 @@
       <c r="G39">
         <v>40</v>
       </c>
-      <c r="N39" s="7"/>
+      <c r="N39" s="6"/>
       <c r="O39">
         <v>6</v>
       </c>
@@ -1437,7 +1443,7 @@
       <c r="G40">
         <v>58</v>
       </c>
-      <c r="N40" s="7"/>
+      <c r="N40" s="6"/>
       <c r="O40">
         <v>7</v>
       </c>
@@ -1455,11 +1461,11 @@
       </c>
     </row>
     <row r="41" spans="2:19">
-      <c r="N41" s="6"/>
+      <c r="N41" s="5"/>
     </row>
     <row r="42" spans="2:19">
-      <c r="C42" s="9" t="s">
-        <v>10</v>
+      <c r="C42" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="F42">
         <v>0.8</v>
@@ -1467,9 +1473,9 @@
       <c r="G42">
         <v>449</v>
       </c>
-      <c r="N42" s="7"/>
-      <c r="O42" s="9" t="s">
-        <v>10</v>
+      <c r="N42" s="6"/>
+      <c r="O42" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="R42">
         <v>0.88</v>
@@ -1479,8 +1485,8 @@
       </c>
     </row>
     <row r="43" spans="2:19">
-      <c r="C43" s="9" t="s">
-        <v>11</v>
+      <c r="C43" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="D43">
         <v>0.82</v>
@@ -1494,9 +1500,9 @@
       <c r="G43">
         <v>449</v>
       </c>
-      <c r="N43" s="7"/>
-      <c r="O43" s="9" t="s">
-        <v>11</v>
+      <c r="N43" s="6"/>
+      <c r="O43" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="P43">
         <v>0.89</v>
@@ -1512,8 +1518,8 @@
       </c>
     </row>
     <row r="44" spans="2:19">
-      <c r="C44" s="9" t="s">
-        <v>12</v>
+      <c r="C44" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="D44">
         <v>0.82</v>
@@ -1527,9 +1533,9 @@
       <c r="G44">
         <v>449</v>
       </c>
-      <c r="N44" s="7"/>
-      <c r="O44" s="9" t="s">
-        <v>12</v>
+      <c r="N44" s="6"/>
+      <c r="O44" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="P44">
         <v>0.9</v>
@@ -1545,39 +1551,39 @@
       </c>
     </row>
     <row r="47" spans="2:19">
-      <c r="B47" s="7"/>
+      <c r="B47" s="6"/>
       <c r="D47" t="s">
+        <v>4</v>
+      </c>
+      <c r="E47" t="s">
+        <v>5</v>
+      </c>
+      <c r="F47" t="s">
         <v>6</v>
       </c>
-      <c r="E47" t="s">
+      <c r="G47" t="s">
         <v>7</v>
       </c>
-      <c r="F47" t="s">
-        <v>8</v>
-      </c>
-      <c r="G47" t="s">
-        <v>9</v>
-      </c>
-      <c r="N47" s="7"/>
+      <c r="N47" s="6"/>
       <c r="P47" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>5</v>
+      </c>
+      <c r="R47" t="s">
         <v>6</v>
       </c>
-      <c r="Q47" t="s">
+      <c r="S47" t="s">
         <v>7</v>
       </c>
-      <c r="R47" t="s">
-        <v>8</v>
-      </c>
-      <c r="S47" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="48" spans="2:19">
-      <c r="B48" s="6"/>
-      <c r="N48" s="6"/>
+      <c r="B48" s="5"/>
+      <c r="N48" s="5"/>
     </row>
     <row r="49" spans="2:19">
-      <c r="B49" s="7"/>
+      <c r="B49" s="6"/>
       <c r="C49">
         <v>0</v>
       </c>
@@ -1593,7 +1599,7 @@
       <c r="G49">
         <v>69</v>
       </c>
-      <c r="N49" s="7"/>
+      <c r="N49" s="6"/>
       <c r="O49">
         <v>0</v>
       </c>
@@ -1611,7 +1617,7 @@
       </c>
     </row>
     <row r="50" spans="2:19">
-      <c r="B50" s="7"/>
+      <c r="B50" s="6"/>
       <c r="C50">
         <v>1</v>
       </c>
@@ -1627,7 +1633,7 @@
       <c r="G50">
         <v>69</v>
       </c>
-      <c r="N50" s="7"/>
+      <c r="N50" s="6"/>
       <c r="O50">
         <v>1</v>
       </c>
@@ -1645,7 +1651,7 @@
       </c>
     </row>
     <row r="51" spans="2:19">
-      <c r="B51" s="7"/>
+      <c r="B51" s="6"/>
       <c r="C51">
         <v>2</v>
       </c>
@@ -1661,7 +1667,7 @@
       <c r="G51">
         <v>57</v>
       </c>
-      <c r="N51" s="7"/>
+      <c r="N51" s="6"/>
       <c r="O51">
         <v>2</v>
       </c>
@@ -1679,7 +1685,7 @@
       </c>
     </row>
     <row r="52" spans="2:19">
-      <c r="B52" s="7"/>
+      <c r="B52" s="6"/>
       <c r="C52">
         <v>3</v>
       </c>
@@ -1695,7 +1701,7 @@
       <c r="G52">
         <v>46</v>
       </c>
-      <c r="N52" s="7"/>
+      <c r="N52" s="6"/>
       <c r="O52">
         <v>3</v>
       </c>
@@ -1713,7 +1719,7 @@
       </c>
     </row>
     <row r="53" spans="2:19">
-      <c r="B53" s="7"/>
+      <c r="B53" s="6"/>
       <c r="C53">
         <v>4</v>
       </c>
@@ -1729,7 +1735,7 @@
       <c r="G53">
         <v>59</v>
       </c>
-      <c r="N53" s="7"/>
+      <c r="N53" s="6"/>
       <c r="O53">
         <v>4</v>
       </c>
@@ -1747,7 +1753,7 @@
       </c>
     </row>
     <row r="54" spans="2:19">
-      <c r="B54" s="7"/>
+      <c r="B54" s="6"/>
       <c r="C54">
         <v>5</v>
       </c>
@@ -1763,7 +1769,7 @@
       <c r="G54">
         <v>49</v>
       </c>
-      <c r="N54" s="7"/>
+      <c r="N54" s="6"/>
       <c r="O54">
         <v>5</v>
       </c>
@@ -1781,7 +1787,7 @@
       </c>
     </row>
     <row r="55" spans="2:19">
-      <c r="B55" s="7"/>
+      <c r="B55" s="6"/>
       <c r="C55">
         <v>6</v>
       </c>
@@ -1797,7 +1803,7 @@
       <c r="G55">
         <v>43</v>
       </c>
-      <c r="N55" s="7"/>
+      <c r="N55" s="6"/>
       <c r="O55">
         <v>6</v>
       </c>
@@ -1815,7 +1821,7 @@
       </c>
     </row>
     <row r="56" spans="2:19">
-      <c r="B56" s="7"/>
+      <c r="B56" s="6"/>
       <c r="C56">
         <v>7</v>
       </c>
@@ -1831,7 +1837,7 @@
       <c r="G56">
         <v>57</v>
       </c>
-      <c r="N56" s="7"/>
+      <c r="N56" s="6"/>
       <c r="O56">
         <v>7</v>
       </c>
@@ -1849,13 +1855,13 @@
       </c>
     </row>
     <row r="57" spans="2:19">
-      <c r="B57" s="6"/>
-      <c r="N57" s="6"/>
+      <c r="B57" s="5"/>
+      <c r="N57" s="5"/>
     </row>
     <row r="58" spans="2:19">
-      <c r="B58" s="7"/>
-      <c r="C58" s="9" t="s">
-        <v>10</v>
+      <c r="B58" s="6"/>
+      <c r="C58" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="F58">
         <v>0.84</v>
@@ -1863,9 +1869,9 @@
       <c r="G58">
         <v>449</v>
       </c>
-      <c r="N58" s="7"/>
-      <c r="O58" s="9" t="s">
-        <v>10</v>
+      <c r="N58" s="6"/>
+      <c r="O58" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="R58">
         <v>0.88</v>
@@ -1875,9 +1881,9 @@
       </c>
     </row>
     <row r="59" spans="2:19">
-      <c r="B59" s="7"/>
-      <c r="C59" s="9" t="s">
-        <v>11</v>
+      <c r="B59" s="6"/>
+      <c r="C59" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="D59">
         <v>0.86</v>
@@ -1891,9 +1897,9 @@
       <c r="G59">
         <v>449</v>
       </c>
-      <c r="N59" s="7"/>
-      <c r="O59" s="9" t="s">
-        <v>11</v>
+      <c r="N59" s="6"/>
+      <c r="O59" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="P59">
         <v>0.88</v>
@@ -1909,9 +1915,9 @@
       </c>
     </row>
     <row r="60" spans="2:19">
-      <c r="B60" s="7"/>
-      <c r="C60" s="9" t="s">
-        <v>12</v>
+      <c r="B60" s="6"/>
+      <c r="C60" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="D60">
         <v>0.85</v>
@@ -1925,9 +1931,9 @@
       <c r="G60">
         <v>449</v>
       </c>
-      <c r="N60" s="7"/>
-      <c r="O60" s="9" t="s">
-        <v>12</v>
+      <c r="N60" s="6"/>
+      <c r="O60" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="P60">
         <v>0.88</v>
@@ -1943,39 +1949,39 @@
       </c>
     </row>
     <row r="63" spans="2:19">
-      <c r="B63" s="7"/>
+      <c r="B63" s="6"/>
       <c r="D63" t="s">
+        <v>4</v>
+      </c>
+      <c r="E63" t="s">
+        <v>5</v>
+      </c>
+      <c r="F63" t="s">
         <v>6</v>
       </c>
-      <c r="E63" t="s">
+      <c r="G63" t="s">
         <v>7</v>
       </c>
-      <c r="F63" t="s">
-        <v>8</v>
-      </c>
-      <c r="G63" t="s">
-        <v>9</v>
-      </c>
-      <c r="N63" s="7"/>
+      <c r="N63" s="6"/>
       <c r="P63" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>5</v>
+      </c>
+      <c r="R63" t="s">
         <v>6</v>
       </c>
-      <c r="Q63" t="s">
+      <c r="S63" t="s">
         <v>7</v>
       </c>
-      <c r="R63" t="s">
-        <v>8</v>
-      </c>
-      <c r="S63" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="64" spans="2:19">
-      <c r="B64" s="6"/>
-      <c r="N64" s="6"/>
+      <c r="B64" s="5"/>
+      <c r="N64" s="5"/>
     </row>
     <row r="65" spans="2:19">
-      <c r="B65" s="7"/>
+      <c r="B65" s="6"/>
       <c r="C65">
         <v>0</v>
       </c>
@@ -1991,7 +1997,7 @@
       <c r="G65">
         <v>60</v>
       </c>
-      <c r="N65" s="7"/>
+      <c r="N65" s="6"/>
       <c r="O65">
         <v>0</v>
       </c>
@@ -2009,7 +2015,7 @@
       </c>
     </row>
     <row r="66" spans="2:19">
-      <c r="B66" s="7"/>
+      <c r="B66" s="6"/>
       <c r="C66">
         <v>1</v>
       </c>
@@ -2025,7 +2031,7 @@
       <c r="G66">
         <v>63</v>
       </c>
-      <c r="N66" s="7"/>
+      <c r="N66" s="6"/>
       <c r="O66">
         <v>1</v>
       </c>
@@ -2043,7 +2049,7 @@
       </c>
     </row>
     <row r="67" spans="2:19">
-      <c r="B67" s="7"/>
+      <c r="B67" s="6"/>
       <c r="C67">
         <v>2</v>
       </c>
@@ -2059,7 +2065,7 @@
       <c r="G67">
         <v>71</v>
       </c>
-      <c r="N67" s="7"/>
+      <c r="N67" s="6"/>
       <c r="O67">
         <v>2</v>
       </c>
@@ -2077,7 +2083,7 @@
       </c>
     </row>
     <row r="68" spans="2:19">
-      <c r="B68" s="7"/>
+      <c r="B68" s="6"/>
       <c r="C68">
         <v>3</v>
       </c>
@@ -2093,7 +2099,7 @@
       <c r="G68">
         <v>47</v>
       </c>
-      <c r="N68" s="7"/>
+      <c r="N68" s="6"/>
       <c r="O68">
         <v>3</v>
       </c>
@@ -2111,7 +2117,7 @@
       </c>
     </row>
     <row r="69" spans="2:19">
-      <c r="B69" s="7"/>
+      <c r="B69" s="6"/>
       <c r="C69">
         <v>4</v>
       </c>
@@ -2127,7 +2133,7 @@
       <c r="G69">
         <v>57</v>
       </c>
-      <c r="N69" s="7"/>
+      <c r="N69" s="6"/>
       <c r="O69">
         <v>4</v>
       </c>
@@ -2145,7 +2151,7 @@
       </c>
     </row>
     <row r="70" spans="2:19">
-      <c r="B70" s="7"/>
+      <c r="B70" s="6"/>
       <c r="C70">
         <v>5</v>
       </c>
@@ -2161,7 +2167,7 @@
       <c r="G70">
         <v>50</v>
       </c>
-      <c r="N70" s="7"/>
+      <c r="N70" s="6"/>
       <c r="O70">
         <v>5</v>
       </c>
@@ -2179,7 +2185,7 @@
       </c>
     </row>
     <row r="71" spans="2:19">
-      <c r="B71" s="7"/>
+      <c r="B71" s="6"/>
       <c r="C71">
         <v>6</v>
       </c>
@@ -2195,7 +2201,7 @@
       <c r="G71">
         <v>41</v>
       </c>
-      <c r="N71" s="7"/>
+      <c r="N71" s="6"/>
       <c r="O71">
         <v>6</v>
       </c>
@@ -2213,7 +2219,7 @@
       </c>
     </row>
     <row r="72" spans="2:19">
-      <c r="B72" s="7"/>
+      <c r="B72" s="6"/>
       <c r="C72">
         <v>7</v>
       </c>
@@ -2229,7 +2235,7 @@
       <c r="G72">
         <v>60</v>
       </c>
-      <c r="N72" s="7"/>
+      <c r="N72" s="6"/>
       <c r="O72">
         <v>7</v>
       </c>
@@ -2247,13 +2253,13 @@
       </c>
     </row>
     <row r="73" spans="2:19">
-      <c r="B73" s="6"/>
-      <c r="N73" s="6"/>
+      <c r="B73" s="5"/>
+      <c r="N73" s="5"/>
     </row>
     <row r="74" spans="2:19">
-      <c r="B74" s="7"/>
-      <c r="C74" s="9" t="s">
-        <v>10</v>
+      <c r="B74" s="6"/>
+      <c r="C74" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="F74">
         <v>0.78</v>
@@ -2261,9 +2267,9 @@
       <c r="G74">
         <v>449</v>
       </c>
-      <c r="N74" s="7"/>
-      <c r="O74" s="9" t="s">
-        <v>10</v>
+      <c r="N74" s="6"/>
+      <c r="O74" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="R74">
         <v>0.8</v>
@@ -2273,9 +2279,9 @@
       </c>
     </row>
     <row r="75" spans="2:19">
-      <c r="B75" s="7"/>
-      <c r="C75" s="9" t="s">
-        <v>11</v>
+      <c r="B75" s="6"/>
+      <c r="C75" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="D75">
         <v>0.79</v>
@@ -2289,9 +2295,9 @@
       <c r="G75">
         <v>449</v>
       </c>
-      <c r="N75" s="7"/>
-      <c r="O75" s="9" t="s">
-        <v>11</v>
+      <c r="N75" s="6"/>
+      <c r="O75" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="P75">
         <v>0.82</v>
@@ -2307,9 +2313,9 @@
       </c>
     </row>
     <row r="76" spans="2:19">
-      <c r="B76" s="7"/>
-      <c r="C76" s="9" t="s">
-        <v>12</v>
+      <c r="B76" s="6"/>
+      <c r="C76" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="D76">
         <v>0.79</v>
@@ -2323,9 +2329,9 @@
       <c r="G76">
         <v>449</v>
       </c>
-      <c r="N76" s="7"/>
-      <c r="O76" s="9" t="s">
-        <v>12</v>
+      <c r="N76" s="6"/>
+      <c r="O76" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="P76">
         <v>0.84</v>
@@ -2342,28 +2348,28 @@
     </row>
     <row r="79" spans="2:19">
       <c r="D79" t="s">
+        <v>4</v>
+      </c>
+      <c r="E79" t="s">
+        <v>5</v>
+      </c>
+      <c r="F79" t="s">
         <v>6</v>
       </c>
-      <c r="E79" t="s">
+      <c r="G79" t="s">
         <v>7</v>
       </c>
-      <c r="F79" t="s">
-        <v>8</v>
-      </c>
-      <c r="G79" t="s">
-        <v>9</v>
-      </c>
       <c r="P79" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q79" t="s">
+        <v>5</v>
+      </c>
+      <c r="R79" t="s">
         <v>6</v>
       </c>
-      <c r="Q79" t="s">
+      <c r="S79" t="s">
         <v>7</v>
-      </c>
-      <c r="R79" t="s">
-        <v>8</v>
-      </c>
-      <c r="S79" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="81" spans="3:19">
@@ -2623,8 +2629,8 @@
       </c>
     </row>
     <row r="90" spans="3:19">
-      <c r="C90" s="9" t="s">
-        <v>10</v>
+      <c r="C90" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="F90">
         <v>0.79</v>
@@ -2632,8 +2638,8 @@
       <c r="G90">
         <v>449</v>
       </c>
-      <c r="O90" s="9" t="s">
-        <v>10</v>
+      <c r="O90" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="R90">
         <v>0.84</v>
@@ -2643,8 +2649,8 @@
       </c>
     </row>
     <row r="91" spans="3:19">
-      <c r="C91" s="9" t="s">
-        <v>11</v>
+      <c r="C91" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="D91">
         <v>0.8</v>
@@ -2658,8 +2664,8 @@
       <c r="G91">
         <v>449</v>
       </c>
-      <c r="O91" s="9" t="s">
-        <v>11</v>
+      <c r="O91" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="P91">
         <v>0.85</v>
@@ -2675,8 +2681,8 @@
       </c>
     </row>
     <row r="92" spans="3:19">
-      <c r="C92" s="9" t="s">
-        <v>12</v>
+      <c r="C92" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="D92">
         <v>0.8</v>
@@ -2690,8 +2696,8 @@
       <c r="G92">
         <v>449</v>
       </c>
-      <c r="O92" s="9" t="s">
-        <v>12</v>
+      <c r="O92" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="P92">
         <v>0.85</v>
@@ -2708,33 +2714,33 @@
     </row>
     <row r="94" spans="3:19">
       <c r="D94" t="s">
+        <v>4</v>
+      </c>
+      <c r="E94" t="s">
+        <v>5</v>
+      </c>
+      <c r="F94" t="s">
         <v>6</v>
       </c>
-      <c r="E94" t="s">
+      <c r="G94" t="s">
         <v>7</v>
       </c>
-      <c r="F94" t="s">
-        <v>8</v>
-      </c>
-      <c r="G94" t="s">
-        <v>9</v>
-      </c>
-      <c r="N94" s="7"/>
+      <c r="N94" s="6"/>
       <c r="P94" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q94" t="s">
+        <v>5</v>
+      </c>
+      <c r="R94" t="s">
         <v>6</v>
       </c>
-      <c r="Q94" t="s">
+      <c r="S94" t="s">
         <v>7</v>
       </c>
-      <c r="R94" t="s">
-        <v>8</v>
-      </c>
-      <c r="S94" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="95" spans="3:19">
-      <c r="N95" s="6"/>
+      <c r="N95" s="5"/>
     </row>
     <row r="96" spans="3:19">
       <c r="C96">
@@ -2752,7 +2758,7 @@
       <c r="G96">
         <v>60</v>
       </c>
-      <c r="N96" s="7"/>
+      <c r="N96" s="6"/>
       <c r="O96">
         <v>0</v>
       </c>
@@ -2785,7 +2791,7 @@
       <c r="G97">
         <v>61</v>
       </c>
-      <c r="N97" s="7"/>
+      <c r="N97" s="6"/>
       <c r="O97">
         <v>1</v>
       </c>
@@ -2818,7 +2824,7 @@
       <c r="G98">
         <v>61</v>
       </c>
-      <c r="N98" s="7"/>
+      <c r="N98" s="6"/>
       <c r="O98">
         <v>2</v>
       </c>
@@ -2851,7 +2857,7 @@
       <c r="G99">
         <v>54</v>
       </c>
-      <c r="N99" s="7"/>
+      <c r="N99" s="6"/>
       <c r="O99">
         <v>3</v>
       </c>
@@ -2884,7 +2890,7 @@
       <c r="G100">
         <v>51</v>
       </c>
-      <c r="N100" s="7"/>
+      <c r="N100" s="6"/>
       <c r="O100">
         <v>4</v>
       </c>
@@ -2917,7 +2923,7 @@
       <c r="G101">
         <v>55</v>
       </c>
-      <c r="N101" s="7"/>
+      <c r="N101" s="6"/>
       <c r="O101">
         <v>5</v>
       </c>
@@ -2950,7 +2956,7 @@
       <c r="G102">
         <v>54</v>
       </c>
-      <c r="N102" s="7"/>
+      <c r="N102" s="6"/>
       <c r="O102">
         <v>6</v>
       </c>
@@ -2983,7 +2989,7 @@
       <c r="G103">
         <v>53</v>
       </c>
-      <c r="N103" s="7"/>
+      <c r="N103" s="6"/>
       <c r="O103">
         <v>7</v>
       </c>
@@ -3001,11 +3007,11 @@
       </c>
     </row>
     <row r="104" spans="3:19">
-      <c r="N104" s="6"/>
+      <c r="N104" s="5"/>
     </row>
     <row r="105" spans="3:19">
-      <c r="C105" s="9" t="s">
-        <v>10</v>
+      <c r="C105" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="F105">
         <v>0.82</v>
@@ -3013,9 +3019,9 @@
       <c r="G105">
         <v>449</v>
       </c>
-      <c r="N105" s="7"/>
-      <c r="O105" s="9" t="s">
-        <v>10</v>
+      <c r="N105" s="6"/>
+      <c r="O105" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="R105">
         <v>0.86</v>
@@ -3025,8 +3031,8 @@
       </c>
     </row>
     <row r="106" spans="3:19">
-      <c r="C106" s="9" t="s">
-        <v>11</v>
+      <c r="C106" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="D106">
         <v>0.83</v>
@@ -3040,9 +3046,9 @@
       <c r="G106">
         <v>449</v>
       </c>
-      <c r="N106" s="7"/>
-      <c r="O106" s="9" t="s">
-        <v>11</v>
+      <c r="N106" s="6"/>
+      <c r="O106" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="P106">
         <v>0.86</v>
@@ -3058,8 +3064,8 @@
       </c>
     </row>
     <row r="107" spans="3:19">
-      <c r="C107" s="9" t="s">
-        <v>12</v>
+      <c r="C107" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="D107">
         <v>0.83</v>
@@ -3073,9 +3079,9 @@
       <c r="G107">
         <v>449</v>
       </c>
-      <c r="N107" s="7"/>
-      <c r="O107" s="9" t="s">
-        <v>12</v>
+      <c r="N107" s="6"/>
+      <c r="O107" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="P107">
         <v>0.87</v>
@@ -3089,6 +3095,69 @@
       <c r="S107">
         <v>218</v>
       </c>
+    </row>
+    <row r="139" spans="5:9">
+      <c r="I139" s="6"/>
+    </row>
+    <row r="140" spans="5:9">
+      <c r="I140" s="6"/>
+    </row>
+    <row r="141" spans="5:9">
+      <c r="I141" s="6"/>
+    </row>
+    <row r="142" spans="5:9">
+      <c r="I142" s="9"/>
+    </row>
+    <row r="143" spans="5:9">
+      <c r="E143" s="6"/>
+      <c r="I143" s="5"/>
+    </row>
+    <row r="144" spans="5:9">
+      <c r="E144" s="6"/>
+      <c r="I144" s="9"/>
+    </row>
+    <row r="145" spans="5:9">
+      <c r="E145" s="6"/>
+      <c r="I145" s="9"/>
+    </row>
+    <row r="146" spans="5:9">
+      <c r="E146" s="6"/>
+      <c r="I146" s="9"/>
+    </row>
+    <row r="147" spans="5:9">
+      <c r="E147" s="6"/>
+      <c r="I147" s="9"/>
+    </row>
+    <row r="148" spans="5:9">
+      <c r="E148" s="6"/>
+      <c r="I148" s="9"/>
+    </row>
+    <row r="149" spans="5:9">
+      <c r="E149" s="6"/>
+      <c r="I149" s="9"/>
+    </row>
+    <row r="150" spans="5:9">
+      <c r="E150" s="6"/>
+      <c r="I150" s="9"/>
+    </row>
+    <row r="151" spans="5:9">
+      <c r="E151" s="5"/>
+      <c r="I151" s="9"/>
+    </row>
+    <row r="152" spans="5:9">
+      <c r="E152" s="6"/>
+      <c r="I152" s="5"/>
+    </row>
+    <row r="153" spans="5:9">
+      <c r="E153" s="6"/>
+      <c r="I153" s="9"/>
+    </row>
+    <row r="154" spans="5:9">
+      <c r="E154" s="6"/>
+      <c r="I154" s="9"/>
+    </row>
+    <row r="155" spans="5:9">
+      <c r="I155" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>